<commit_message>
all data mapped in grid
</commit_message>
<xml_diff>
--- a/errorData.xlsx
+++ b/errorData.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -22,6 +22,9 @@
     <t>Age</t>
   </si>
   <si>
+    <t>Att</t>
+  </si>
+  <si>
     <t>Attendance</t>
   </si>
   <si>
@@ -46,10 +49,7 @@
     <t>Virat</t>
   </si>
   <si>
-    <t>77y</t>
-  </si>
-  <si>
-    <t>rina</t>
+    <t>Parker</t>
   </si>
   <si>
     <t>null</t>
@@ -58,7 +58,22 @@
     <t>undefined</t>
   </si>
   <si>
-    <t>eeeeeee</t>
+    <t>olive</t>
+  </si>
+  <si>
+    <t>Tim</t>
+  </si>
+  <si>
+    <t>Stocks</t>
+  </si>
+  <si>
+    <t>Trucker</t>
+  </si>
+  <si>
+    <t>Hennesy</t>
+  </si>
+  <si>
+    <t>Tim Rose</t>
   </si>
 </sst>
 </file>
@@ -96,12 +111,16 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -335,10 +354,13 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1">
         <v>10.0</v>
@@ -347,12 +369,15 @@
         <v>16.0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E2" s="3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1">
         <v>9.0</v>
@@ -361,12 +386,15 @@
         <v>15.0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1">
         <v>10.0</v>
@@ -375,12 +403,15 @@
         <v>17.0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E4" s="3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1">
         <v>10.0</v>
@@ -389,12 +420,15 @@
         <v>16.0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1">
         <v>9.0</v>
@@ -403,15 +437,27 @@
         <v>14.0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="B7" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>17.0</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -424,7 +470,10 @@
       <c r="C8" s="1">
         <v>15.0</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -432,7 +481,13 @@
       <c r="A9" s="1">
         <v>12.0</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -447,12 +502,15 @@
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E10" s="3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1">
         <v>10.0</v>
@@ -461,12 +519,15 @@
         <v>17.0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E11" s="3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B12" s="1">
         <v>10.0</v>
@@ -475,12 +536,15 @@
         <v>16.0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E12" s="3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1">
         <v>9.0</v>
@@ -489,7 +553,10 @@
         <v>14.0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="14">
@@ -503,7 +570,10 @@
         <v>14</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="15">
@@ -516,8 +586,110 @@
       <c r="C15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>13</v>
+      <c r="D15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>16.0</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="C17" s="1">
+        <v>17.0</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="C18" s="1">
+        <v>13.0</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="C19" s="1">
+        <v>16.0</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="C20" s="1">
+        <v>18.0</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="D21" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>4.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>